<commit_message>
Add employees template. Reformat all excel templates to STM style
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF98A9E-494E-42F2-9DBC-5BA7AEB18A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4586CB0-DF6C-4638-8D37-E83F32140DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Отпуска" sheetId="1" r:id="rId1"/>
+    <sheet name="Сотрудники" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="W6")</t>
+jx:area(lastCell="W5")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="W6")</t>
+jx:each(items="employees" var="e" lastCell="W5" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -105,12 +105,6 @@
     <t>${e.displayName}</t>
   </si>
   <si>
-    <t>${e.employeeCurrentProject}</t>
-  </si>
-  <si>
-    <t>${e.currentProjectId}</t>
-  </si>
-  <si>
     <t>Телефон</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>Выгрузка сотрудников компании из системы HR Easy</t>
+  </si>
+  <si>
+    <t>${e.currentProject}</t>
+  </si>
+  <si>
+    <t>${e.email}</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -353,11 +353,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -383,21 +405,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -421,22 +428,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>204788</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2486025</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:colOff>2200275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1162051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
+        <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCBD5E8-98AB-4F02-9390-F1142A2B6993}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{739A42FA-8F50-4F8A-9033-B721F77E7BC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -444,16 +451,15 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="2979" t="8904" r="4679" b="13698"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="204788"/>
-          <a:ext cx="2219325" cy="1143000"/>
+          <a:off x="133350" y="85725"/>
+          <a:ext cx="2066925" cy="1076326"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -466,19 +472,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A4:W5" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A4:W5" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A4:W5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:W5">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Уровень экспертизы"/>
     <tableColumn id="10" xr3:uid="{DA50F1B3-475E-4D76-9C0A-64F0B8D65742}" name="Рабочее место"/>
@@ -494,7 +500,7 @@
     <tableColumn id="20" xr3:uid="{A17EE04E-E8C8-477E-AF16-C735D4063995}" name="Семейный статус"/>
     <tableColumn id="21" xr3:uid="{79B291B5-5726-498B-B004-5B1A54643FBC}" name="Загранпаспорт"/>
     <tableColumn id="22" xr3:uid="{3EC984DC-1A99-4FDD-BEFC-E6ADF5BBF9E7}" name="Уровень английского"/>
-    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения"/>
+    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,40 +830,40 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.59765625" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" customWidth="1"/>
-    <col min="4" max="4" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.86328125" customWidth="1"/>
-    <col min="9" max="9" width="22.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.1328125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="29.1328125" customWidth="1"/>
-    <col min="13" max="13" width="11.1328125" customWidth="1"/>
-    <col min="14" max="14" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.3984375" customWidth="1"/>
-    <col min="16" max="16" width="14.1328125" customWidth="1"/>
-    <col min="17" max="17" width="16.3984375" customWidth="1"/>
-    <col min="18" max="18" width="22.73046875" customWidth="1"/>
-    <col min="19" max="19" width="25.73046875" customWidth="1"/>
-    <col min="20" max="20" width="23.86328125" customWidth="1"/>
-    <col min="21" max="21" width="27.3984375" customWidth="1"/>
-    <col min="22" max="22" width="26.86328125" customWidth="1"/>
-    <col min="23" max="23" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+    <col min="19" max="19" width="25.7109375" customWidth="1"/>
+    <col min="20" max="20" width="23.85546875" customWidth="1"/>
+    <col min="21" max="21" width="27.42578125" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="99" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -881,7 +887,8 @@
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
@@ -909,8 +916,32 @@
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
     </row>
-    <row r="3" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -921,135 +952,135 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="S5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="T5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="V5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W5" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +1100,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Some cosmetics changes in templates
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4586CB0-DF6C-4638-8D37-E83F32140DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999A6D7-EA2C-4B88-B982-53860B0D0820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,11 +52,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="W5")</t>
+jx:area(lastCell="W4")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="W5" orderBy="displayName")</t>
+jx:each(items="employees" var="e" lastCell="W4" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -428,15 +428,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2200275</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1162051</xdr:rowOff>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -458,8 +458,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="133350" y="85725"/>
-          <a:ext cx="2066925" cy="1076326"/>
+          <a:off x="504825" y="0"/>
+          <a:ext cx="1590675" cy="828325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -472,10 +472,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A4:W5" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A4:W5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:W5">
-    <sortCondition ref="A4:A5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:W4" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A3:W4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W4">
+    <sortCondition ref="A3:A4"/>
   </sortState>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
@@ -827,10 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +861,7 @@
     <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>46</v>
@@ -916,170 +917,145 @@
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
     </row>
-    <row r="3" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J4" t="s">
         <v>45</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K4" t="s">
         <v>44</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L4" t="s">
         <v>43</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M4" t="s">
         <v>42</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N4" t="s">
         <v>41</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O4" t="s">
         <v>40</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P4" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q4" t="s">
         <v>38</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R4" t="s">
         <v>37</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S4" t="s">
         <v>36</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T4" t="s">
         <v>35</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U4" t="s">
         <v>34</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V4" t="s">
         <v>33</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add business account to employee export table
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999A6D7-EA2C-4B88-B982-53860B0D0820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AD17A3-A701-4138-B392-7ED09AD0057C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="W4")</t>
+jx:area(lastCell="X4")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="W4" orderBy="displayName")</t>
+jx:each(items="employees" var="e" lastCell="X4" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ФИО</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>${e.email}</t>
+  </si>
+  <si>
+    <t>${e.ba}</t>
+  </si>
+  <si>
+    <t>Бизнес аккаунт</t>
   </si>
 </sst>
 </file>
@@ -358,7 +364,10 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -472,19 +481,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:W4" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A3:W4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:X4" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A3:X4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="23">
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Уровень экспертизы"/>
     <tableColumn id="10" xr3:uid="{DA50F1B3-475E-4D76-9C0A-64F0B8D65742}" name="Рабочее место"/>
@@ -500,7 +510,7 @@
     <tableColumn id="20" xr3:uid="{A17EE04E-E8C8-477E-AF16-C735D4063995}" name="Семейный статус"/>
     <tableColumn id="21" xr3:uid="{79B291B5-5726-498B-B004-5B1A54643FBC}" name="Загранпаспорт"/>
     <tableColumn id="22" xr3:uid="{3EC984DC-1A99-4FDD-BEFC-E6ADF5BBF9E7}" name="Уровень английского"/>
-    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -827,41 +837,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="29.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.7109375" customWidth="1"/>
-    <col min="20" max="20" width="23.85546875" customWidth="1"/>
-    <col min="21" max="21" width="27.42578125" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" customWidth="1"/>
-    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" customWidth="1"/>
+    <col min="22" max="22" width="27.42578125" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>46</v>
@@ -887,8 +897,9 @@
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
@@ -896,7 +907,7 @@
       <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -916,8 +927,9 @@
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
     </row>
-    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -928,67 +940,70 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -999,63 +1014,66 @@
         <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>45</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>42</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>41</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>40</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>38</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>37</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>36</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>35</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>34</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>33</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add telegram to admin page and excel export
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AD17A3-A701-4138-B392-7ED09AD0057C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4ED91D-2C70-48CD-AACC-EFE79B7420BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="X4")</t>
+jx:area(lastCell="Y4")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="X4" orderBy="displayName")</t>
+jx:each(items="employees" var="e" lastCell="Y4" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ФИО</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Бизнес аккаунт</t>
+  </si>
+  <si>
+    <t>Telegram</t>
+  </si>
+  <si>
+    <t>${e.telegram}</t>
   </si>
 </sst>
 </file>
@@ -364,7 +370,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -382,6 +388,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -481,18 +490,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:X4" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A3:X4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:Y4" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A3:Y4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="24">
+  <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="4"/>
+    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
@@ -837,11 +847,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,28 +860,28 @@
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" customWidth="1"/>
-    <col min="20" max="20" width="25.7109375" customWidth="1"/>
-    <col min="21" max="21" width="23.85546875" customWidth="1"/>
-    <col min="22" max="22" width="27.42578125" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="29.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" customWidth="1"/>
+    <col min="21" max="21" width="25.7109375" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" customWidth="1"/>
+    <col min="23" max="23" width="27.42578125" customWidth="1"/>
+    <col min="24" max="24" width="26.85546875" customWidth="1"/>
+    <col min="25" max="25" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>46</v>
@@ -898,8 +908,9 @@
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
@@ -928,8 +939,9 @@
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -949,61 +961,64 @@
         <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1022,58 +1037,61 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>45</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>44</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>43</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>42</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>41</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>39</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>38</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>37</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>36</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>35</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>34</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="Y4" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Do not show employee's skills and current project role without special permissions
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4ED91D-2C70-48CD-AACC-EFE79B7420BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D0E74E-B5F3-4EC3-B7F9-4337BDB97D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="Y4")</t>
+jx:area(lastCell="Z4")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="Y4" orderBy="displayName")</t>
+jx:each(items="employees" var="e" lastCell="Z4" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ФИО</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>${e.telegram}</t>
+  </si>
+  <si>
+    <t>Роль на проекте</t>
+  </si>
+  <si>
+    <t>${e.currentProjectRole}</t>
   </si>
 </sst>
 </file>
@@ -370,7 +376,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -382,6 +388,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -490,19 +499,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:Y4" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A3:Y4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:Z4" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:Z4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Z4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="25">
+  <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{2CF1E783-42FA-435B-A9B0-71CCC889D77B}" name="Роль на проекте" dataDxfId="0"/>
+    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
@@ -847,41 +857,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="21" customWidth="1"/>
-    <col min="14" max="14" width="29.140625" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" customWidth="1"/>
-    <col min="21" max="21" width="25.7109375" customWidth="1"/>
-    <col min="22" max="22" width="23.85546875" customWidth="1"/>
-    <col min="23" max="23" width="27.42578125" customWidth="1"/>
-    <col min="24" max="24" width="26.85546875" customWidth="1"/>
-    <col min="25" max="25" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="17" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" customWidth="1"/>
+    <col min="24" max="24" width="27.42578125" customWidth="1"/>
+    <col min="25" max="25" width="26.85546875" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>46</v>
@@ -909,8 +919,9 @@
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
@@ -919,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -940,8 +951,9 @@
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -952,73 +964,76 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1029,69 +1044,72 @@
         <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>43</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>40</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>39</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>38</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>37</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>36</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>35</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>34</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>33</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Z4" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Do not show employee's skills and current project role without special permissions (#41)
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4ED91D-2C70-48CD-AACC-EFE79B7420BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D0E74E-B5F3-4EC3-B7F9-4337BDB97D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="Y4")</t>
+jx:area(lastCell="Z4")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="Y4" orderBy="displayName")</t>
+jx:each(items="employees" var="e" lastCell="Z4" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ФИО</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>${e.telegram}</t>
+  </si>
+  <si>
+    <t>Роль на проекте</t>
+  </si>
+  <si>
+    <t>${e.currentProjectRole}</t>
   </si>
 </sst>
 </file>
@@ -370,7 +376,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -382,6 +388,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -490,19 +499,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:Y4" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A3:Y4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:Z4" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:Z4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Z4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="25">
+  <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{2CF1E783-42FA-435B-A9B0-71CCC889D77B}" name="Роль на проекте" dataDxfId="0"/>
+    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
@@ -847,41 +857,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="21" customWidth="1"/>
-    <col min="14" max="14" width="29.140625" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" customWidth="1"/>
-    <col min="21" max="21" width="25.7109375" customWidth="1"/>
-    <col min="22" max="22" width="23.85546875" customWidth="1"/>
-    <col min="23" max="23" width="27.42578125" customWidth="1"/>
-    <col min="24" max="24" width="26.85546875" customWidth="1"/>
-    <col min="25" max="25" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="17" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" customWidth="1"/>
+    <col min="24" max="24" width="27.42578125" customWidth="1"/>
+    <col min="25" max="25" width="26.85546875" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>46</v>
@@ -909,8 +919,9 @@
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
@@ -919,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -940,8 +951,9 @@
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -952,73 +964,76 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1029,69 +1044,72 @@
         <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>43</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>40</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>39</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>38</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>37</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>36</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>35</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>34</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>33</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Z4" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add organization field to employee
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D0E74E-B5F3-4EC3-B7F9-4337BDB97D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91722F4F-F34A-4AA3-AF6D-9FC2785A2629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Сотрудники" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -42,7 +42,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Автор:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="Z4")</t>
+jx:area(lastCell="AA4")</t>
         </r>
       </text>
     </comment>
@@ -66,7 +66,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Автор:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>ФИО</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>${e.currentProjectRole}</t>
+  </si>
+  <si>
+    <t>Организация</t>
+  </si>
+  <si>
+    <t>${e.organization}</t>
   </si>
 </sst>
 </file>
@@ -374,29 +380,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -499,22 +505,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:Z4" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:Z4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Z4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:AA4" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:AA4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AA4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="26">
+  <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{2CF1E783-42FA-435B-A9B0-71CCC889D77B}" name="Роль на проекте" dataDxfId="0"/>
-    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="5"/>
-    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{2CF1E783-42FA-435B-A9B0-71CCC889D77B}" name="Роль на проекте" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="4"/>
+    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Уровень экспертизы"/>
     <tableColumn id="10" xr3:uid="{DA50F1B3-475E-4D76-9C0A-64F0B8D65742}" name="Рабочее место"/>
@@ -525,21 +531,22 @@
     <tableColumn id="15" xr3:uid="{AAC3EF14-AB7F-4E28-B27A-D4BB5C3FEED4}" name="Рабочий день"/>
     <tableColumn id="16" xr3:uid="{B39AB8F8-F9A7-44C7-BB9F-896266D2AF17}" name="Место работы"/>
     <tableColumn id="17" xr3:uid="{A01D1389-5397-4C6B-AA32-26C10078A9E2}" name="Подразделение"/>
+    <tableColumn id="28" xr3:uid="{E988AACC-D8EB-49F8-8FB3-B8D353A4293E}" name="Организация"/>
     <tableColumn id="18" xr3:uid="{C27F935E-18D9-4D42-8EF2-7F711FFE8654}" name="Город проживания"/>
     <tableColumn id="19" xr3:uid="{2C11CA5F-E5AC-4676-8068-44894FCD3D15}" name="Дети"/>
     <tableColumn id="20" xr3:uid="{A17EE04E-E8C8-477E-AF16-C735D4063995}" name="Семейный статус"/>
     <tableColumn id="21" xr3:uid="{79B291B5-5726-498B-B004-5B1A54643FBC}" name="Загранпаспорт"/>
     <tableColumn id="22" xr3:uid="{3EC984DC-1A99-4FDD-BEFC-E6ADF5BBF9E7}" name="Уровень английского"/>
-    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -577,9 +584,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,26 +619,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -664,26 +654,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -857,11 +830,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +864,7 @@
     <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>46</v>
@@ -921,7 +894,7 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="9" t="s">
         <v>1</v>
@@ -953,7 +926,7 @@
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1015,25 +988,28 @@
         <v>25</v>
       </c>
       <c r="U3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1095,21 +1071,24 @@
         <v>38</v>
       </c>
       <c r="U4" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" t="s">
         <v>37</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>36</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>35</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>34</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>33</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="AA4" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add organization to employees table, form, excel
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_employees_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_employees_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91722F4F-F34A-4AA3-AF6D-9FC2785A2629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873A185E-000B-4844-9EB0-EB38AC64A977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Сотрудники" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>Автор</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -42,7 +42,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Автор:</t>
         </r>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="e" lastCell="Z4" orderBy="displayName")</t>
+jx:each(items="employees" var="e" lastCell="AA4" orderBy="displayName")</t>
         </r>
       </text>
     </comment>
@@ -380,26 +380,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -505,22 +508,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:AA4" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A3:AA4" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A3:AA4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AA4">
     <sortCondition ref="A3:A4"/>
   </sortState>
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ФИО"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{2CF1E783-42FA-435B-A9B0-71CCC889D77B}" name="Роль на проекте" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Skype" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Текущий проект" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{2CF1E783-42FA-435B-A9B0-71CCC889D77B}" name="Роль на проекте" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{D293F5E8-02A4-47F1-A8B5-1446B2110421}" name="Бизнес аккаунт" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Телефон" dataDxfId="6"/>
+    <tableColumn id="25" xr3:uid="{3DBEBAD8-1961-454B-AB1D-54B4D3044F8A}" name="Telegram" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{10B83D6D-F71C-42A9-9640-B2DC46318818}" name="Подразделение" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{4E765C0B-EC7F-4DD0-9E45-AA769E6594A7}" name="Организация" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Дата трудоустройства" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="День рождения" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Позиция"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Уровень экспертизы"/>
     <tableColumn id="10" xr3:uid="{DA50F1B3-475E-4D76-9C0A-64F0B8D65742}" name="Рабочее место"/>
@@ -530,14 +534,13 @@
     <tableColumn id="14" xr3:uid="{C544F49F-228C-43BC-A19B-2358B1C43905}" name="ФИО супруга/супруги"/>
     <tableColumn id="15" xr3:uid="{AAC3EF14-AB7F-4E28-B27A-D4BB5C3FEED4}" name="Рабочий день"/>
     <tableColumn id="16" xr3:uid="{B39AB8F8-F9A7-44C7-BB9F-896266D2AF17}" name="Место работы"/>
-    <tableColumn id="17" xr3:uid="{A01D1389-5397-4C6B-AA32-26C10078A9E2}" name="Подразделение"/>
-    <tableColumn id="28" xr3:uid="{E988AACC-D8EB-49F8-8FB3-B8D353A4293E}" name="Организация"/>
     <tableColumn id="18" xr3:uid="{C27F935E-18D9-4D42-8EF2-7F711FFE8654}" name="Город проживания"/>
     <tableColumn id="19" xr3:uid="{2C11CA5F-E5AC-4676-8068-44894FCD3D15}" name="Дети"/>
     <tableColumn id="20" xr3:uid="{A17EE04E-E8C8-477E-AF16-C735D4063995}" name="Семейный статус"/>
     <tableColumn id="21" xr3:uid="{79B291B5-5726-498B-B004-5B1A54643FBC}" name="Загранпаспорт"/>
     <tableColumn id="22" xr3:uid="{3EC984DC-1A99-4FDD-BEFC-E6ADF5BBF9E7}" name="Уровень английского"/>
-    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="0"/>
+    <tableColumn id="28" xr3:uid="{AC770C52-4960-4CFD-B50D-CFB1613486F1}" name="Skype"/>
+    <tableColumn id="23" xr3:uid="{13E7F2B1-140C-43F9-AD05-47E67B04BB41}" name="Дата увольнения" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -832,23 +835,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
     <col min="14" max="14" width="21" customWidth="1"/>
     <col min="15" max="15" width="29.140625" customWidth="1"/>
     <col min="16" max="16" width="11.140625" customWidth="1"/>
@@ -856,12 +860,10 @@
     <col min="18" max="18" width="16.42578125" customWidth="1"/>
     <col min="19" max="19" width="14.140625" customWidth="1"/>
     <col min="20" max="20" width="16.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22.7109375" customWidth="1"/>
-    <col min="22" max="22" width="25.7109375" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" customWidth="1"/>
-    <col min="24" max="24" width="27.42578125" customWidth="1"/>
-    <col min="25" max="25" width="26.85546875" customWidth="1"/>
-    <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" customWidth="1"/>
+    <col min="22" max="22" width="27.42578125" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,8 +893,6 @@
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -923,8 +923,6 @@
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -946,64 +944,64 @@
         <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="AA3" s="4" t="s">
         <v>31</v>
@@ -1029,64 +1027,64 @@
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z4" t="s">
         <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U4" t="s">
-        <v>56</v>
-      </c>
-      <c r="V4" t="s">
-        <v>37</v>
-      </c>
-      <c r="W4" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>33</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>32</v>

</xml_diff>